<commit_message>
update nach gespräch 23_02
</commit_message>
<xml_diff>
--- a/Results_comp.xlsx
+++ b/Results_comp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\OneDrive\Dokumente\GitHub\MA-pre-work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e6b024c9cb94357/Dokumente/GitHub/MA-pre-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28D44724-9F0C-42C7-AC27-00BBE808AD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{28D44724-9F0C-42C7-AC27-00BBE808AD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{257790E9-2A3B-46B1-BDE7-17E608B32223}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3A20839C-8FC4-4563-A5AC-03E15566398E}"/>
   </bookViews>
@@ -16,42 +16,15 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$C$7:$C$39</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$C$7:$C$36</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$D$6</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Tabelle1!$D$6</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Tabelle1!$D$7:$D$39</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Tabelle1!$E$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Tabelle1!$E$7:$E$39</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Tabelle1!$F$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Tabelle1!$F$7:$F$39</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Tabelle1!$G$6</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Tabelle1!$G$7:$G$39</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Tabelle1!$C$7:$C$39</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Tabelle1!$D$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$D$7:$D$39</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Tabelle1!$D$7:$D$39</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Tabelle1!$E$6</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Tabelle1!$E$7:$E$39</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Tabelle1!$F$6</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Tabelle1!$F$7:$F$39</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Tabelle1!$G$6</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Tabelle1!$G$7:$G$39</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Tabelle1!$C$7:$C$38</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Tabelle1!$D$6</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Tabelle1!$D$7:$D$38</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$D$7:$D$36</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Tabelle1!$E$6</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Tabelle1!$E$6</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Tabelle1!$E$7:$E$38</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Tabelle1!$F$6</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Tabelle1!$F$7:$F$38</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Tabelle1!$G$6</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$G$7:$G$38</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$E$7:$E$39</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$E$7:$E$36</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Tabelle1!$F$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Tabelle1!$F$7:$F$39</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Tabelle1!$F$7:$F$36</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Tabelle1!$G$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Tabelle1!$G$7:$G$39</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Tabelle1!$C$7:$C$39</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Tabelle1!$G$7:$G$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Results first generation of Triplet contrastive Model and Autoencoder comparision to Superviesed Modell:</t>
   </si>
@@ -115,29 +88,139 @@
     <t>Random Seed 96:</t>
   </si>
   <si>
-    <t>Contrastive_Self-Supervised_try_1</t>
-  </si>
-  <si>
-    <t>Contrastive_Self-Supervised</t>
-  </si>
-  <si>
-    <t>Contrastive_Self-Supervised_try_2</t>
-  </si>
-  <si>
-    <t>Autoencoder_Self-Supervised_try_1</t>
-  </si>
-  <si>
-    <t>Autoencoder_Self-Supervised</t>
-  </si>
-  <si>
-    <t>Autoencoder_Self-Supervised_try_2</t>
+    <t>Mean Supervised</t>
+  </si>
+  <si>
+    <t>Mean Contrastive</t>
+  </si>
+  <si>
+    <t>Mean Autoencoder</t>
+  </si>
+  <si>
+    <t>Accuracy:</t>
+  </si>
+  <si>
+    <t>Triplet_loss_Self-Supervised_try_1</t>
+  </si>
+  <si>
+    <t>Triplet_loss_Self-Supervised</t>
+  </si>
+  <si>
+    <t>Triplet_loss_Self-Supervised_try_2</t>
+  </si>
+  <si>
+    <t>MAE_Self-Supervised_try_1</t>
+  </si>
+  <si>
+    <t>MAE_Self-Supervised</t>
+  </si>
+  <si>
+    <t>MAE_Self-Supervised_try_2</t>
+  </si>
+  <si>
+    <t>SA-Model:</t>
+  </si>
+  <si>
+    <t>Time/freq Mask 7/50 default,
+ batch size =  32S, 
+desired length =  15 sec</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Test1: masking</t>
+  </si>
+  <si>
+    <t>Test2: masking</t>
+  </si>
+  <si>
+    <t>Test3: batchsize</t>
+  </si>
+  <si>
+    <t>Time/freq Mask 7/50 default,
+ batch size =  16, 
+desired length =  15 sec</t>
+  </si>
+  <si>
+    <t>Time/freq Mask 7/50 default,
+ batch size =  8, 
+desired length =  15 sec</t>
+  </si>
+  <si>
+    <t>Test4: batchsize</t>
+  </si>
+  <si>
+    <t>Test5: Single  connected layer</t>
+  </si>
+  <si>
+    <t>Standalone Tests:</t>
+  </si>
+  <si>
+    <t>Comparision Refrence Models:</t>
+  </si>
+  <si>
+    <t>Standalone Model:</t>
+  </si>
+  <si>
+    <t>Reference Run 1:</t>
+  </si>
+  <si>
+    <t>Reference Run 2:</t>
+  </si>
+  <si>
+    <t>Reference Run 3:</t>
+  </si>
+  <si>
+    <t>Reference Run 4:</t>
+  </si>
+  <si>
+    <t>Reference Run 5:</t>
+  </si>
+  <si>
+    <t>2-Phase Model: Triplet Model</t>
+  </si>
+  <si>
+    <t>2-Phase Model: Autoencoder Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2</t>
+  </si>
+  <si>
+    <t>Test6: Length shortage</t>
+  </si>
+  <si>
+    <t>Time/freq Mask 7/50 default,
+ batch size =  32, 
+desired length =  7 sec</t>
+  </si>
+  <si>
+    <t>Time/freq Mask 7/50 default,
+ batch size =  32, 
+desired length =  15 sec</t>
+  </si>
+  <si>
+    <t>Time/freq NO Mask ,
+ batch size =  32, 
+desired length =  15 sec</t>
+  </si>
+  <si>
+    <t>Time/freq 30/120 Mask ,
+ batch size =  32, 
+desired length =  15 sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +230,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,13 +262,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -323,7 +430,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling min="0.80000000000000004"/>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -893,15 +1000,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>766984</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>27609</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>101601</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>160130</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>88348</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -937,8 +1044,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1171575" y="7791450"/>
-              <a:ext cx="6321426" cy="4749800"/>
+              <a:off x="3097434" y="7546009"/>
+              <a:ext cx="6289246" cy="4296189"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -957,9 +1064,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="de-AT" sz="1100"/>
-                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
-Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -971,10 +1078,29 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E127AD73-D5D8-4CCF-84C8-A2807AFB030F}" name="Table3" displayName="Table3" ref="A77:F84" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A77:F84" xr:uid="{E127AD73-D5D8-4CCF-84C8-A2807AFB030F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{AB8CDC6F-9C20-4096-A0E5-0D72E0B4664E}" name=" "/>
+    <tableColumn id="2" xr3:uid="{C0AC0F0D-6EDE-47BC-8E7D-486DB954E22B}" name=" 2" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{99D3A78A-7368-42C8-93BF-F875498BBB3C}" name="macro avg f1"/>
+    <tableColumn id="4" xr3:uid="{7F7018A6-5984-424B-92B1-0A1D2415EAFE}" name="macro avg-precision/balanced Accuracy"/>
+    <tableColumn id="5" xr3:uid="{5ABB6AD2-F7EC-4A30-AB50-8C9516D2D242}" name="Kappa"/>
+    <tableColumn id="6" xr3:uid="{9EA54D08-66EF-44C3-879C-A916CE98A696}" name="Accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1012,7 +1138,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1118,7 +1244,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1260,7 +1386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1268,32 +1394,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA59E500-7BAA-4205-AA8D-1B424910C6AC}">
-  <dimension ref="A2:G39"/>
+  <dimension ref="A2:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" customWidth="1"/>
     <col min="2" max="2" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1310,12 +1439,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>0.94</v>
@@ -1330,12 +1459,12 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>0.94</v>
@@ -1350,262 +1479,326 @@
         <v>0.95340000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0.89</v>
+      </c>
+      <c r="E9">
+        <v>0.88</v>
+      </c>
+      <c r="F9">
+        <v>0.88590000000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>0.91</v>
+      </c>
+      <c r="E10">
+        <v>0.89</v>
+      </c>
+      <c r="F10">
+        <v>0.88539999999999996</v>
+      </c>
+      <c r="G10">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0.88</v>
+      </c>
+      <c r="E11">
+        <v>0.87</v>
+      </c>
+      <c r="F11">
+        <v>0.85140000000000005</v>
+      </c>
+      <c r="G11">
+        <v>0.90680000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>0.88</v>
+      </c>
+      <c r="E12">
+        <v>0.86</v>
+      </c>
+      <c r="F12">
+        <v>0.86129999999999995</v>
+      </c>
+      <c r="G12">
+        <v>0.91310000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="D9">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
         <v>0.88</v>
       </c>
-      <c r="E9">
+      <c r="E15">
         <v>0.87</v>
       </c>
-      <c r="F9">
-        <v>0.85140000000000005</v>
-      </c>
-      <c r="G9">
-        <v>0.90680000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+      <c r="F15">
+        <v>0.87660000000000005</v>
+      </c>
+      <c r="G15">
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>0.88</v>
-      </c>
-      <c r="E10">
-        <v>0.86</v>
-      </c>
-      <c r="F10">
-        <v>0.86129999999999995</v>
-      </c>
-      <c r="G10">
-        <v>0.91310000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
+      <c r="D16">
         <v>0.89</v>
       </c>
-      <c r="E11">
-        <v>0.88</v>
-      </c>
-      <c r="F11">
-        <v>0.88590000000000002</v>
-      </c>
-      <c r="G11">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>0.91</v>
-      </c>
-      <c r="E12">
+      <c r="E16">
         <v>0.89</v>
       </c>
-      <c r="F12">
-        <v>0.88539999999999996</v>
-      </c>
-      <c r="G12">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16">
-        <v>0.88</v>
-      </c>
-      <c r="E16">
-        <v>0.87</v>
-      </c>
       <c r="F16">
-        <v>0.87660000000000005</v>
+        <v>0.87970000000000004</v>
       </c>
       <c r="G16">
-        <v>0.92159999999999997</v>
+        <v>0.92369999999999997</v>
+      </c>
+      <c r="J16" s="1">
+        <f>AVERAGE(G9:G10,G17:G18,G25:G26,G33:G34)</f>
+        <v>0.92401250000000001</v>
+      </c>
+      <c r="K16" s="1">
+        <f>AVERAGE(G7:G8,G15:G16,G23:G24,G31:G32)</f>
+        <v>0.93854999999999988</v>
+      </c>
+      <c r="L16" s="1">
+        <f>AVERAGE(G11:G12,G19:G20,G27:G28,G35:G36)</f>
+        <v>0.90995000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="E17">
-        <v>0.89</v>
+        <v>0.86719999999999997</v>
       </c>
       <c r="F17">
-        <v>0.87970000000000004</v>
+        <v>0.86629999999999996</v>
       </c>
       <c r="G17">
-        <v>0.92369999999999997</v>
+        <v>0.9153</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="E18">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="F18">
-        <v>0.85629999999999995</v>
+        <v>0.86639999999999995</v>
       </c>
       <c r="G18">
-        <v>0.90890000000000004</v>
+        <v>0.9153</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="E19">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="F19">
-        <v>0.82509999999999994</v>
+        <v>0.85629999999999995</v>
       </c>
       <c r="G19">
-        <v>0.88980000000000004</v>
+        <v>0.90890000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="E20">
-        <v>0.86719999999999997</v>
+        <v>0.89</v>
       </c>
       <c r="F20">
-        <v>0.86629999999999996</v>
+        <v>0.82509999999999994</v>
       </c>
       <c r="G20">
-        <v>0.9153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21">
-        <v>0.89</v>
-      </c>
-      <c r="E21">
-        <v>0.88</v>
-      </c>
-      <c r="F21">
-        <v>0.86639999999999995</v>
-      </c>
-      <c r="G21">
-        <v>0.9153</v>
+        <v>0.88980000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>0.94</v>
+      </c>
+      <c r="E23">
+        <v>0.95</v>
+      </c>
+      <c r="F23">
+        <v>0.89980000000000004</v>
+      </c>
+      <c r="G23">
+        <v>0.93640000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>12</v>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>0.93</v>
+      </c>
+      <c r="E24">
+        <v>0.93</v>
+      </c>
+      <c r="F24">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="G24">
+        <v>0.94069999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="E25">
-        <v>0.95</v>
+        <v>0.89</v>
       </c>
       <c r="F25">
-        <v>0.89980000000000004</v>
+        <v>0.88190000000000002</v>
       </c>
       <c r="G25">
-        <v>0.93640000000000001</v>
+        <v>0.92579999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="E26">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="F26">
-        <v>0.90600000000000003</v>
+        <v>0.88849999999999996</v>
       </c>
       <c r="G26">
-        <v>0.94069999999999998</v>
+        <v>0.93010000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D27">
         <v>0.87</v>
@@ -1622,10 +1815,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D28">
         <v>0.86</v>
@@ -1640,174 +1833,363 @@
         <v>0.90039999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>0.93</v>
+      </c>
+      <c r="E31">
+        <v>0.92</v>
+      </c>
+      <c r="F31">
+        <v>0.91310000000000002</v>
+      </c>
+      <c r="G31">
+        <v>0.94489999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>0.92</v>
+      </c>
+      <c r="E32">
+        <v>0.92</v>
+      </c>
+      <c r="F32">
+        <v>0.90620000000000001</v>
+      </c>
+      <c r="G32">
+        <v>0.94069999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C33" t="s">
         <v>11</v>
       </c>
-      <c r="D29">
+      <c r="D33">
+        <v>0.91</v>
+      </c>
+      <c r="E33">
         <v>0.89</v>
       </c>
-      <c r="E29">
+      <c r="F33">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="G33">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>0.91</v>
+      </c>
+      <c r="E34">
+        <v>0.9</v>
+      </c>
+      <c r="F34">
+        <v>0.87709999999999999</v>
+      </c>
+      <c r="G34">
+        <v>0.92159999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35">
         <v>0.89</v>
       </c>
-      <c r="F29">
-        <v>0.88190000000000002</v>
-      </c>
-      <c r="G29">
-        <v>0.92579999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <v>0.9</v>
-      </c>
-      <c r="E30">
-        <v>0.9</v>
-      </c>
-      <c r="F30">
-        <v>0.88849999999999996</v>
-      </c>
-      <c r="G30">
-        <v>0.93010000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34">
-        <v>0.93</v>
-      </c>
-      <c r="E34">
-        <v>0.92</v>
-      </c>
-      <c r="F34">
-        <v>0.91310000000000002</v>
-      </c>
-      <c r="G34">
-        <v>0.94489999999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <v>0.92</v>
-      </c>
       <c r="E35">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="F35">
-        <v>0.90620000000000001</v>
+        <v>0.87980000000000003</v>
       </c>
       <c r="G35">
-        <v>0.94069999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.92369999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D36">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="E36">
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="F36">
-        <v>0.87980000000000003</v>
+        <v>0.85150000000000003</v>
       </c>
       <c r="G36">
-        <v>0.92369999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37">
-        <v>0.84</v>
-      </c>
-      <c r="E37">
-        <v>0.84</v>
-      </c>
-      <c r="F37">
-        <v>0.85150000000000003</v>
-      </c>
-      <c r="G37">
         <v>0.90680000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38">
-        <v>0.91</v>
-      </c>
-      <c r="E38">
-        <v>0.89</v>
-      </c>
-      <c r="F38">
-        <v>0.88639999999999997</v>
-      </c>
-      <c r="G38">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39">
-        <v>0.91</v>
-      </c>
-      <c r="E39">
-        <v>0.9</v>
-      </c>
-      <c r="F39">
-        <v>0.87709999999999999</v>
-      </c>
-      <c r="G39">
-        <v>0.92159999999999997</v>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>